<commit_message>
final edit to presentation
</commit_message>
<xml_diff>
--- a/data/Presentation.xlsx
+++ b/data/Presentation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boourns\Documents\NSS\projects\app-trader-team_whatsapp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boourns\Documents\NSS\projects\app-trader-team_whatsapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD747FDE-C48A-44E2-A60D-28F1BF130DDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41613CDB-AF26-4895-8874-12FC1273E40F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F2CD9FB3-B309-4415-AF1A-9A3FBD712EDA}"/>
   </bookViews>
@@ -443,6 +443,30 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -481,30 +505,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2346,6 +2346,71 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="10000"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+          <c:dispUnitsLbl>
+            <c:layout>
+              <c:manualLayout>
+                <c:xMode val="edge"/>
+                <c:yMode val="edge"/>
+                <c:x val="4.0240825688073398E-2"/>
+                <c:y val="0.39160621180650185"/>
+              </c:manualLayout>
+            </c:layout>
+            <c:tx>
+              <c:rich>
+                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US"/>
+                    <a:t>(n Millions)</a:t>
+                  </a:r>
+                </a:p>
+              </c:rich>
+            </c:tx>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2765,6 +2830,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Count of Apps</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2904,7 +3024,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t>) </a:t>
+              <a:t> </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2970,6 +3090,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -3275,7 +3396,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" b="1" baseline="0"/>
-                  <a:t> Counts(Billions)</a:t>
+                  <a:t> Counts (Billions)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" b="1"/>
               </a:p>
@@ -3344,6 +3465,9 @@
         <c:crossAx val="442188992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="billions"/>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -5258,37 +5382,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -9731,7 +9824,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="1">
           <cell r="D1" t="str">
@@ -9868,7 +9961,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -9884,7 +9977,7 @@
       <sheetName val="genres_installs"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="30">
           <cell r="I30" t="str">
@@ -10516,8 +10609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F350FD5-83D1-49C2-AA50-01D8A3BFFCF2}">
   <dimension ref="B132:H193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G183" sqref="G183"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F190" sqref="F190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10786,84 +10879,84 @@
       </c>
     </row>
     <row r="144" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="G144" s="13" t="s">
+      <c r="G144" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H144" s="14"/>
+      <c r="H144" s="22"/>
     </row>
     <row r="145" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G145" s="15"/>
-      <c r="H145" s="16"/>
+      <c r="G145" s="23"/>
+      <c r="H145" s="24"/>
     </row>
     <row r="146" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="147" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B147" s="17" t="s">
+      <c r="B147" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C147" s="18"/>
-      <c r="D147" s="18"/>
-      <c r="E147" s="18"/>
-      <c r="F147" s="18"/>
-      <c r="G147" s="18"/>
-      <c r="H147" s="19"/>
+      <c r="C147" s="26"/>
+      <c r="D147" s="26"/>
+      <c r="E147" s="26"/>
+      <c r="F147" s="26"/>
+      <c r="G147" s="26"/>
+      <c r="H147" s="27"/>
     </row>
     <row r="148" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B148" s="20"/>
-      <c r="C148" s="21"/>
-      <c r="D148" s="21"/>
-      <c r="E148" s="21"/>
-      <c r="F148" s="21"/>
-      <c r="G148" s="21"/>
-      <c r="H148" s="22"/>
+      <c r="B148" s="28"/>
+      <c r="C148" s="29"/>
+      <c r="D148" s="29"/>
+      <c r="E148" s="29"/>
+      <c r="F148" s="29"/>
+      <c r="G148" s="29"/>
+      <c r="H148" s="30"/>
     </row>
     <row r="149" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B149" s="20"/>
-      <c r="C149" s="21"/>
-      <c r="D149" s="21"/>
-      <c r="E149" s="21"/>
-      <c r="F149" s="21"/>
-      <c r="G149" s="21"/>
-      <c r="H149" s="22"/>
+      <c r="B149" s="28"/>
+      <c r="C149" s="29"/>
+      <c r="D149" s="29"/>
+      <c r="E149" s="29"/>
+      <c r="F149" s="29"/>
+      <c r="G149" s="29"/>
+      <c r="H149" s="30"/>
     </row>
     <row r="150" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B150" s="20"/>
-      <c r="C150" s="21"/>
-      <c r="D150" s="21"/>
-      <c r="E150" s="21"/>
-      <c r="F150" s="21"/>
-      <c r="G150" s="21"/>
-      <c r="H150" s="22"/>
+      <c r="B150" s="28"/>
+      <c r="C150" s="29"/>
+      <c r="D150" s="29"/>
+      <c r="E150" s="29"/>
+      <c r="F150" s="29"/>
+      <c r="G150" s="29"/>
+      <c r="H150" s="30"/>
     </row>
     <row r="151" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B151" s="20"/>
-      <c r="C151" s="21"/>
-      <c r="D151" s="21"/>
-      <c r="E151" s="21"/>
-      <c r="F151" s="21"/>
-      <c r="G151" s="21"/>
-      <c r="H151" s="22"/>
+      <c r="B151" s="28"/>
+      <c r="C151" s="29"/>
+      <c r="D151" s="29"/>
+      <c r="E151" s="29"/>
+      <c r="F151" s="29"/>
+      <c r="G151" s="29"/>
+      <c r="H151" s="30"/>
     </row>
     <row r="152" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B152" s="23"/>
-      <c r="C152" s="24"/>
-      <c r="D152" s="24"/>
-      <c r="E152" s="24"/>
-      <c r="F152" s="24"/>
-      <c r="G152" s="24"/>
-      <c r="H152" s="25"/>
+      <c r="B152" s="31"/>
+      <c r="C152" s="32"/>
+      <c r="D152" s="32"/>
+      <c r="E152" s="32"/>
+      <c r="F152" s="32"/>
+      <c r="G152" s="32"/>
+      <c r="H152" s="33"/>
     </row>
     <row r="181" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="182" spans="2:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B182" s="31" t="s">
+      <c r="B182" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C182" s="31" t="s">
+      <c r="C182" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D182" s="31" t="s">
+      <c r="D182" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E182" s="31" t="s">
+      <c r="E182" s="18" t="s">
         <v>19</v>
       </c>
       <c r="G182" s="34" t="s">
@@ -10875,19 +10968,19 @@
       <c r="B183" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C183" s="32">
+      <c r="C183" s="19">
         <v>226.32985776954197</v>
       </c>
-      <c r="D183" s="26">
+      <c r="D183" s="13">
         <v>565824.64442385489</v>
       </c>
-      <c r="E183" s="27">
+      <c r="E183" s="14">
         <v>67898957.330862582</v>
       </c>
       <c r="G183" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H183" s="27">
+      <c r="H183" s="14">
         <v>5000</v>
       </c>
     </row>
@@ -10895,19 +10988,19 @@
       <c r="B184" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C184" s="32">
+      <c r="C184" s="19">
         <v>218.36868624623935</v>
       </c>
-      <c r="D184" s="26">
+      <c r="D184" s="13">
         <v>545921.71561559837</v>
       </c>
-      <c r="E184" s="27">
+      <c r="E184" s="14">
         <v>65510605.873871803</v>
       </c>
       <c r="G184" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H184" s="27">
+      <c r="H184" s="14">
         <v>1500</v>
       </c>
     </row>
@@ -10915,19 +11008,19 @@
       <c r="B185" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C185" s="32">
+      <c r="C185" s="19">
         <v>216.07941348135586</v>
       </c>
-      <c r="D185" s="26">
+      <c r="D185" s="13">
         <v>540198.53370338969</v>
       </c>
-      <c r="E185" s="27">
+      <c r="E185" s="14">
         <v>64823824.044406772</v>
       </c>
       <c r="G185" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H185" s="27">
+      <c r="H185" s="14">
         <f>1500*7*12</f>
         <v>126000</v>
       </c>
@@ -10936,19 +11029,19 @@
       <c r="B186" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C186" s="32">
+      <c r="C186" s="19">
         <v>207.69978702632056</v>
       </c>
-      <c r="D186" s="26">
+      <c r="D186" s="13">
         <v>519249.4675658014</v>
       </c>
-      <c r="E186" s="27">
+      <c r="E186" s="14">
         <v>56078942.497106552</v>
       </c>
       <c r="G186" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H186" s="29">
+      <c r="H186" s="16">
         <v>1260000</v>
       </c>
     </row>
@@ -10956,13 +11049,13 @@
       <c r="B187" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C187" s="32">
+      <c r="C187" s="19">
         <v>193.23490842076012</v>
       </c>
-      <c r="D187" s="26">
+      <c r="D187" s="13">
         <v>483087.27105190029</v>
       </c>
-      <c r="E187" s="27">
+      <c r="E187" s="14">
         <v>52173425.273605235</v>
       </c>
     </row>
@@ -10970,13 +11063,13 @@
       <c r="B188" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C188" s="32">
+      <c r="C188" s="19">
         <v>193.06283266780778</v>
       </c>
-      <c r="D188" s="26">
+      <c r="D188" s="13">
         <v>482657.08166951948</v>
       </c>
-      <c r="E188" s="27">
+      <c r="E188" s="14">
         <v>52126964.820308104</v>
       </c>
     </row>
@@ -10984,13 +11077,13 @@
       <c r="B189" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C189" s="32">
+      <c r="C189" s="19">
         <v>171.61029095391532</v>
       </c>
-      <c r="D189" s="26">
+      <c r="D189" s="13">
         <v>429025.72738478833</v>
       </c>
-      <c r="E189" s="27">
+      <c r="E189" s="14">
         <v>41186469.828939676</v>
       </c>
     </row>
@@ -10998,13 +11091,13 @@
       <c r="B190" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C190" s="32">
+      <c r="C190" s="19">
         <v>112.51409148370948</v>
       </c>
-      <c r="D190" s="26">
+      <c r="D190" s="13">
         <v>281285.22870927368</v>
       </c>
-      <c r="E190" s="27">
+      <c r="E190" s="14">
         <v>33754227.445112839</v>
       </c>
     </row>
@@ -11012,13 +11105,13 @@
       <c r="B191" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C191" s="32">
+      <c r="C191" s="19">
         <v>109.18982944419598</v>
       </c>
-      <c r="D191" s="26">
+      <c r="D191" s="13">
         <v>272974.57361048996</v>
       </c>
-      <c r="E191" s="27">
+      <c r="E191" s="14">
         <v>32756948.833258793</v>
       </c>
     </row>
@@ -11026,18 +11119,18 @@
       <c r="B192" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C192" s="33">
+      <c r="C192" s="20">
         <v>108.86794157143667</v>
       </c>
-      <c r="D192" s="28">
+      <c r="D192" s="15">
         <v>272169.85392859171</v>
       </c>
-      <c r="E192" s="29">
+      <c r="E192" s="16">
         <v>32660382.471431006</v>
       </c>
     </row>
     <row r="193" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E193" s="30">
+      <c r="E193" s="17">
         <v>498970748.41890335</v>
       </c>
     </row>

</xml_diff>